<commit_message>
Docs(Update): relocated tabel in Gantt chart, added various content to informations via links to external Websites to document and started a todo-list.
</commit_message>
<xml_diff>
--- a/Dokumente/Projektablauf_Gantt.xlsx
+++ b/Dokumente/Projektablauf_Gantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yvesj\OneDrive - Kt. SG BLD (1)\Schule_IMS-T1a\000_IMS\001-IntegriertePraxisarbeit\2025_TerminalChat\Dokumente\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bldsg-my.sharepoint.com/personal/yves_jaros_edu_gbssg_ch/Documents/000_Schule_IMS-T1a/000_IMS/001-IntegriertePraxisarbeit/2025_TerminalChat/Dokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E4EBFE-A1CD-4CA4-901D-6FF22ED8BFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{D7E4EBFE-A1CD-4CA4-901D-6FF22ED8BFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDC1F04E-2C9F-4470-979B-30A8E973D01A}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -765,15 +765,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -800,6 +791,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1086,263 +1086,369 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:BB48"/>
+  <dimension ref="A1:AZ46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="12.85546875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="12" hidden="1" customWidth="1"/>
-    <col min="12" max="14" width="12.42578125" hidden="1" customWidth="1"/>
-    <col min="15" max="17" width="12.85546875" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="28" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="32" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="40" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="49" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="54" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="51" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="41" t="s">
+    <row r="1" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G3" s="29">
+      <c r="E1" s="29">
         <v>45719</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="F1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="G1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="H1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="30" t="s">
+      <c r="I1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="30" t="s">
+      <c r="J1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="30" t="s">
+      <c r="K1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="30" t="s">
+      <c r="L1" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="M1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="30" t="s">
+      <c r="N1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="30" t="s">
+      <c r="O1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Y3" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AB3" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AC3" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AE3" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AG3" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AH3" s="8" t="s">
+      <c r="AF1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AI3" s="8" t="s">
+      <c r="AG1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AJ3" s="8" t="s">
+      <c r="AH1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AK3" s="8" t="s">
+      <c r="AI1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AL3" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AM3" s="8" t="s">
+      <c r="AK1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AN3" s="8" t="s">
+      <c r="AL1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AO3" s="8" t="s">
+      <c r="AM1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AP3" s="8" t="s">
+      <c r="AN1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="AQ3" s="8" t="s">
+      <c r="AO1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AR3" s="8" t="s">
+      <c r="AP1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AS3" s="8" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AT3" s="8" t="s">
+      <c r="AR1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AU3" s="8" t="s">
+      <c r="AS1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AV3" s="8" t="s">
+      <c r="AT1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AW3" s="8" t="s">
+      <c r="AU1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AX3" s="8" t="s">
+      <c r="AV1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AY3" s="8" t="s">
+      <c r="AW1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AZ3" s="8" t="s">
+      <c r="AX1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="BA3" s="8" t="s">
+      <c r="AY1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="BB3" s="9" t="s">
+      <c r="AZ1" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="3:54" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="42" t="s">
+    <row r="2" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="20"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="20"/>
-      <c r="AB4" s="20"/>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="20"/>
-      <c r="AE4" s="20"/>
-      <c r="AF4" s="20"/>
-      <c r="AG4" s="20"/>
-      <c r="AH4" s="20"/>
-      <c r="AI4" s="20"/>
-      <c r="AJ4" s="20"/>
-      <c r="AK4" s="20"/>
-      <c r="AL4" s="20"/>
-      <c r="AM4" s="20"/>
-      <c r="AN4" s="20"/>
-      <c r="AO4" s="20"/>
-      <c r="AP4" s="20"/>
-      <c r="AQ4" s="20"/>
-      <c r="AR4" s="20"/>
-      <c r="AS4" s="20"/>
-      <c r="AT4" s="20"/>
-      <c r="AU4" s="20"/>
-      <c r="AV4" s="20"/>
-      <c r="AW4" s="20"/>
-      <c r="AX4" s="20"/>
-      <c r="AY4" s="20"/>
-      <c r="AZ4" s="20"/>
-      <c r="BA4" s="20"/>
-      <c r="BB4" s="31" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AL2" s="20"/>
+      <c r="AM2" s="20"/>
+      <c r="AN2" s="20"/>
+      <c r="AO2" s="20"/>
+      <c r="AP2" s="20"/>
+      <c r="AQ2" s="20"/>
+      <c r="AR2" s="20"/>
+      <c r="AS2" s="20"/>
+      <c r="AT2" s="20"/>
+      <c r="AU2" s="20"/>
+      <c r="AV2" s="20"/>
+      <c r="AW2" s="20"/>
+      <c r="AX2" s="20"/>
+      <c r="AY2" s="20"/>
+      <c r="AZ2" s="42" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C5" s="43" t="s">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="B3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="4"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="43"/>
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="2"/>
+      <c r="AU4" s="2"/>
+      <c r="AV4" s="2"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="2"/>
+      <c r="AZ4" s="43"/>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1387,20 +1493,20 @@
       <c r="AW5" s="2"/>
       <c r="AX5" s="2"/>
       <c r="AY5" s="2"/>
-      <c r="AZ5" s="2"/>
-      <c r="BA5" s="2"/>
-      <c r="BB5" s="32"/>
-    </row>
-    <row r="6" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C6" s="43" t="s">
+      <c r="AZ5" s="43"/>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A6" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="4"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1445,20 +1551,20 @@
       <c r="AW6" s="2"/>
       <c r="AX6" s="2"/>
       <c r="AY6" s="2"/>
-      <c r="AZ6" s="2"/>
-      <c r="BA6" s="2"/>
-      <c r="BB6" s="32"/>
-    </row>
-    <row r="7" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C7" s="43" t="s">
+      <c r="AZ6" s="43"/>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="4"/>
+      <c r="B7" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1503,20 +1609,22 @@
       <c r="AW7" s="2"/>
       <c r="AX7" s="2"/>
       <c r="AY7" s="2"/>
-      <c r="AZ7" s="2"/>
-      <c r="BA7" s="2"/>
-      <c r="BB7" s="32"/>
-    </row>
-    <row r="8" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C8" s="43" t="s">
+      <c r="AZ7" s="43"/>
+    </row>
+    <row r="8" spans="1:52" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="4"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1561,20 +1669,20 @@
       <c r="AW8" s="2"/>
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
-      <c r="AZ8" s="2"/>
-      <c r="BA8" s="2"/>
-      <c r="BB8" s="32"/>
-    </row>
-    <row r="9" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C9" s="43" t="s">
+      <c r="AZ8" s="43"/>
+    </row>
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1619,22 +1727,20 @@
       <c r="AW9" s="2"/>
       <c r="AX9" s="2"/>
       <c r="AY9" s="2"/>
-      <c r="AZ9" s="2"/>
-      <c r="BA9" s="2"/>
-      <c r="BB9" s="32"/>
-    </row>
-    <row r="10" spans="3:54" ht="45" x14ac:dyDescent="0.25">
-      <c r="C10" s="43" t="s">
+      <c r="AZ9" s="43"/>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A10" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" s="4"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1679,20 +1785,20 @@
       <c r="AW10" s="2"/>
       <c r="AX10" s="2"/>
       <c r="AY10" s="2"/>
-      <c r="AZ10" s="2"/>
-      <c r="BA10" s="2"/>
-      <c r="BB10" s="32"/>
-    </row>
-    <row r="11" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C11" s="43" t="s">
+      <c r="AZ10" s="43"/>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="4"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1737,20 +1843,20 @@
       <c r="AW11" s="2"/>
       <c r="AX11" s="2"/>
       <c r="AY11" s="2"/>
-      <c r="AZ11" s="2"/>
-      <c r="BA11" s="2"/>
-      <c r="BB11" s="32"/>
-    </row>
-    <row r="12" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C12" s="43" t="s">
+      <c r="AZ11" s="43"/>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A12" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="4"/>
+      <c r="B12" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1795,20 +1901,20 @@
       <c r="AW12" s="2"/>
       <c r="AX12" s="2"/>
       <c r="AY12" s="2"/>
-      <c r="AZ12" s="2"/>
-      <c r="BA12" s="2"/>
-      <c r="BB12" s="32"/>
-    </row>
-    <row r="13" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C13" s="43" t="s">
+      <c r="AZ12" s="43"/>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A13" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="4"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1853,78 +1959,76 @@
       <c r="AW13" s="2"/>
       <c r="AX13" s="2"/>
       <c r="AY13" s="2"/>
-      <c r="AZ13" s="2"/>
-      <c r="BA13" s="2"/>
-      <c r="BB13" s="32"/>
-    </row>
-    <row r="14" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C14" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2"/>
-      <c r="Y14" s="2"/>
-      <c r="Z14" s="2"/>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="2"/>
-      <c r="AC14" s="2"/>
-      <c r="AD14" s="2"/>
-      <c r="AE14" s="2"/>
-      <c r="AF14" s="2"/>
-      <c r="AG14" s="2"/>
-      <c r="AH14" s="2"/>
-      <c r="AI14" s="2"/>
-      <c r="AJ14" s="2"/>
-      <c r="AK14" s="2"/>
-      <c r="AL14" s="2"/>
-      <c r="AM14" s="2"/>
-      <c r="AN14" s="2"/>
-      <c r="AO14" s="2"/>
-      <c r="AP14" s="2"/>
-      <c r="AQ14" s="2"/>
-      <c r="AR14" s="2"/>
-      <c r="AS14" s="2"/>
-      <c r="AT14" s="2"/>
-      <c r="AU14" s="2"/>
-      <c r="AV14" s="2"/>
-      <c r="AW14" s="2"/>
-      <c r="AX14" s="2"/>
-      <c r="AY14" s="2"/>
-      <c r="AZ14" s="2"/>
-      <c r="BA14" s="2"/>
-      <c r="BB14" s="32"/>
-    </row>
-    <row r="15" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C15" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="4"/>
+      <c r="AZ13" s="43"/>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A14" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="33"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="24"/>
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="24"/>
+      <c r="AB14" s="24"/>
+      <c r="AC14" s="24"/>
+      <c r="AD14" s="24"/>
+      <c r="AE14" s="24"/>
+      <c r="AF14" s="24"/>
+      <c r="AG14" s="24"/>
+      <c r="AH14" s="24"/>
+      <c r="AI14" s="24"/>
+      <c r="AJ14" s="24"/>
+      <c r="AK14" s="24"/>
+      <c r="AL14" s="24"/>
+      <c r="AM14" s="24"/>
+      <c r="AN14" s="24"/>
+      <c r="AO14" s="24"/>
+      <c r="AP14" s="24"/>
+      <c r="AQ14" s="24"/>
+      <c r="AR14" s="24"/>
+      <c r="AS14" s="24"/>
+      <c r="AT14" s="24"/>
+      <c r="AU14" s="24"/>
+      <c r="AV14" s="24"/>
+      <c r="AW14" s="24"/>
+      <c r="AX14" s="24"/>
+      <c r="AY14" s="24"/>
+      <c r="AZ14" s="43"/>
+    </row>
+    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A15" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1969,76 +2073,82 @@
       <c r="AW15" s="2"/>
       <c r="AX15" s="2"/>
       <c r="AY15" s="2"/>
-      <c r="AZ15" s="2"/>
-      <c r="BA15" s="2"/>
-      <c r="BB15" s="32"/>
-    </row>
-    <row r="16" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C16" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="24"/>
-      <c r="Z16" s="24"/>
-      <c r="AA16" s="24"/>
-      <c r="AB16" s="24"/>
-      <c r="AC16" s="24"/>
-      <c r="AD16" s="24"/>
-      <c r="AE16" s="24"/>
-      <c r="AF16" s="24"/>
-      <c r="AG16" s="24"/>
-      <c r="AH16" s="24"/>
-      <c r="AI16" s="24"/>
-      <c r="AJ16" s="24"/>
-      <c r="AK16" s="24"/>
-      <c r="AL16" s="24"/>
-      <c r="AM16" s="24"/>
-      <c r="AN16" s="24"/>
-      <c r="AO16" s="24"/>
-      <c r="AP16" s="24"/>
-      <c r="AQ16" s="24"/>
-      <c r="AR16" s="24"/>
-      <c r="AS16" s="24"/>
-      <c r="AT16" s="24"/>
-      <c r="AU16" s="24"/>
-      <c r="AV16" s="24"/>
-      <c r="AW16" s="24"/>
-      <c r="AX16" s="24"/>
-      <c r="AY16" s="24"/>
-      <c r="AZ16" s="24"/>
-      <c r="BA16" s="24"/>
-      <c r="BB16" s="32"/>
-    </row>
-    <row r="17" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C17" s="43" t="s">
+      <c r="AZ15" s="43"/>
+    </row>
+    <row r="16" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="4"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="2"/>
+      <c r="AN16" s="2"/>
+      <c r="AO16" s="2"/>
+      <c r="AP16" s="2"/>
+      <c r="AQ16" s="2"/>
+      <c r="AR16" s="2"/>
+      <c r="AS16" s="2"/>
+      <c r="AT16" s="2"/>
+      <c r="AU16" s="2"/>
+      <c r="AV16" s="2"/>
+      <c r="AW16" s="2"/>
+      <c r="AX16" s="2"/>
+      <c r="AY16" s="2"/>
+      <c r="AZ16" s="43"/>
+    </row>
+    <row r="17" spans="1:52" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -2083,22 +2193,22 @@
       <c r="AW17" s="2"/>
       <c r="AX17" s="2"/>
       <c r="AY17" s="2"/>
-      <c r="AZ17" s="2"/>
-      <c r="BA17" s="2"/>
-      <c r="BB17" s="32"/>
-    </row>
-    <row r="18" spans="3:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="C18" s="43" t="s">
+      <c r="AZ17" s="43"/>
+    </row>
+    <row r="18" spans="1:52" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="G18" s="4"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -2143,22 +2253,22 @@
       <c r="AW18" s="2"/>
       <c r="AX18" s="2"/>
       <c r="AY18" s="2"/>
-      <c r="AZ18" s="2"/>
-      <c r="BA18" s="2"/>
-      <c r="BB18" s="32"/>
-    </row>
-    <row r="19" spans="3:54" ht="60" x14ac:dyDescent="0.25">
-      <c r="C19" s="43" t="s">
+      <c r="AZ18" s="43"/>
+    </row>
+    <row r="19" spans="1:52" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="G19" s="4"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -2203,22 +2313,20 @@
       <c r="AW19" s="2"/>
       <c r="AX19" s="2"/>
       <c r="AY19" s="2"/>
-      <c r="AZ19" s="2"/>
-      <c r="BA19" s="2"/>
-      <c r="BB19" s="32"/>
-    </row>
-    <row r="20" spans="3:54" ht="45" x14ac:dyDescent="0.25">
-      <c r="C20" s="43" t="s">
+      <c r="AZ19" s="43"/>
+    </row>
+    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A20" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" s="4"/>
+      <c r="B20" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -2263,22 +2371,22 @@
       <c r="AW20" s="2"/>
       <c r="AX20" s="2"/>
       <c r="AY20" s="2"/>
-      <c r="AZ20" s="2"/>
-      <c r="BA20" s="2"/>
-      <c r="BB20" s="32"/>
-    </row>
-    <row r="21" spans="3:54" ht="45" x14ac:dyDescent="0.25">
-      <c r="C21" s="43" t="s">
+      <c r="AZ20" s="43"/>
+    </row>
+    <row r="21" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="4"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -2323,20 +2431,20 @@
       <c r="AW21" s="2"/>
       <c r="AX21" s="2"/>
       <c r="AY21" s="2"/>
-      <c r="AZ21" s="2"/>
-      <c r="BA21" s="2"/>
-      <c r="BB21" s="32"/>
-    </row>
-    <row r="22" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C22" s="43" t="s">
+      <c r="AZ21" s="43"/>
+    </row>
+    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A22" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="4"/>
+      <c r="B22" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -2381,22 +2489,22 @@
       <c r="AW22" s="2"/>
       <c r="AX22" s="2"/>
       <c r="AY22" s="2"/>
-      <c r="AZ22" s="2"/>
-      <c r="BA22" s="2"/>
-      <c r="BB22" s="32"/>
-    </row>
-    <row r="23" spans="3:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="C23" s="43" t="s">
+      <c r="AZ22" s="43"/>
+    </row>
+    <row r="23" spans="1:52" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="35"/>
-      <c r="E23" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" s="4"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -2441,20 +2549,22 @@
       <c r="AW23" s="2"/>
       <c r="AX23" s="2"/>
       <c r="AY23" s="2"/>
-      <c r="AZ23" s="2"/>
-      <c r="BA23" s="2"/>
-      <c r="BB23" s="32"/>
-    </row>
-    <row r="24" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C24" s="43" t="s">
+      <c r="AZ23" s="43"/>
+    </row>
+    <row r="24" spans="1:52" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="4"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2499,22 +2609,22 @@
       <c r="AW24" s="2"/>
       <c r="AX24" s="2"/>
       <c r="AY24" s="2"/>
-      <c r="AZ24" s="2"/>
-      <c r="BA24" s="2"/>
-      <c r="BB24" s="32"/>
-    </row>
-    <row r="25" spans="3:54" ht="45" x14ac:dyDescent="0.25">
-      <c r="C25" s="43" t="s">
+      <c r="AZ24" s="43"/>
+    </row>
+    <row r="25" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G25" s="4"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2559,22 +2669,22 @@
       <c r="AW25" s="2"/>
       <c r="AX25" s="2"/>
       <c r="AY25" s="2"/>
-      <c r="AZ25" s="2"/>
-      <c r="BA25" s="2"/>
-      <c r="BB25" s="32"/>
-    </row>
-    <row r="26" spans="3:54" ht="60" x14ac:dyDescent="0.25">
-      <c r="C26" s="43" t="s">
+      <c r="AZ25" s="43"/>
+    </row>
+    <row r="26" spans="1:52" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G26" s="4"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -2619,82 +2729,76 @@
       <c r="AW26" s="2"/>
       <c r="AX26" s="2"/>
       <c r="AY26" s="2"/>
-      <c r="AZ26" s="2"/>
-      <c r="BA26" s="2"/>
-      <c r="BB26" s="32"/>
-    </row>
-    <row r="27" spans="3:54" ht="30" x14ac:dyDescent="0.25">
-      <c r="C27" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="35"/>
-      <c r="E27" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
-      <c r="X27" s="2"/>
-      <c r="Y27" s="2"/>
-      <c r="Z27" s="2"/>
-      <c r="AA27" s="2"/>
-      <c r="AB27" s="2"/>
-      <c r="AC27" s="2"/>
-      <c r="AD27" s="2"/>
-      <c r="AE27" s="2"/>
-      <c r="AF27" s="2"/>
-      <c r="AG27" s="2"/>
-      <c r="AH27" s="2"/>
-      <c r="AI27" s="2"/>
-      <c r="AJ27" s="2"/>
-      <c r="AK27" s="2"/>
-      <c r="AL27" s="2"/>
-      <c r="AM27" s="2"/>
-      <c r="AN27" s="2"/>
-      <c r="AO27" s="2"/>
-      <c r="AP27" s="2"/>
-      <c r="AQ27" s="2"/>
-      <c r="AR27" s="2"/>
-      <c r="AS27" s="2"/>
-      <c r="AT27" s="2"/>
-      <c r="AU27" s="2"/>
-      <c r="AV27" s="2"/>
-      <c r="AW27" s="2"/>
-      <c r="AX27" s="2"/>
-      <c r="AY27" s="2"/>
-      <c r="AZ27" s="2"/>
-      <c r="BA27" s="2"/>
-      <c r="BB27" s="32"/>
-    </row>
-    <row r="28" spans="3:54" ht="45" x14ac:dyDescent="0.25">
-      <c r="C28" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="G28" s="4"/>
+      <c r="AZ26" s="43"/>
+    </row>
+    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A27" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="24"/>
+      <c r="R27" s="24"/>
+      <c r="S27" s="24"/>
+      <c r="T27" s="24"/>
+      <c r="U27" s="24"/>
+      <c r="V27" s="24"/>
+      <c r="W27" s="24"/>
+      <c r="X27" s="24"/>
+      <c r="Y27" s="24"/>
+      <c r="Z27" s="24"/>
+      <c r="AA27" s="24"/>
+      <c r="AB27" s="24"/>
+      <c r="AC27" s="24"/>
+      <c r="AD27" s="24"/>
+      <c r="AE27" s="24"/>
+      <c r="AF27" s="24"/>
+      <c r="AG27" s="24"/>
+      <c r="AH27" s="24"/>
+      <c r="AI27" s="24"/>
+      <c r="AJ27" s="24"/>
+      <c r="AK27" s="24"/>
+      <c r="AL27" s="24"/>
+      <c r="AM27" s="24"/>
+      <c r="AN27" s="24"/>
+      <c r="AO27" s="24"/>
+      <c r="AP27" s="24"/>
+      <c r="AQ27" s="24"/>
+      <c r="AR27" s="24"/>
+      <c r="AS27" s="24"/>
+      <c r="AT27" s="24"/>
+      <c r="AU27" s="24"/>
+      <c r="AV27" s="24"/>
+      <c r="AW27" s="24"/>
+      <c r="AX27" s="24"/>
+      <c r="AY27" s="24"/>
+      <c r="AZ27" s="43"/>
+    </row>
+    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A28" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -2739,76 +2843,78 @@
       <c r="AW28" s="2"/>
       <c r="AX28" s="2"/>
       <c r="AY28" s="2"/>
-      <c r="AZ28" s="2"/>
-      <c r="BA28" s="2"/>
-      <c r="BB28" s="32"/>
-    </row>
-    <row r="29" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C29" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="36"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="24"/>
-      <c r="U29" s="24"/>
-      <c r="V29" s="24"/>
-      <c r="W29" s="24"/>
-      <c r="X29" s="24"/>
-      <c r="Y29" s="24"/>
-      <c r="Z29" s="24"/>
-      <c r="AA29" s="24"/>
-      <c r="AB29" s="24"/>
-      <c r="AC29" s="24"/>
-      <c r="AD29" s="24"/>
-      <c r="AE29" s="24"/>
-      <c r="AF29" s="24"/>
-      <c r="AG29" s="24"/>
-      <c r="AH29" s="24"/>
-      <c r="AI29" s="24"/>
-      <c r="AJ29" s="24"/>
-      <c r="AK29" s="24"/>
-      <c r="AL29" s="24"/>
-      <c r="AM29" s="24"/>
-      <c r="AN29" s="24"/>
-      <c r="AO29" s="24"/>
-      <c r="AP29" s="24"/>
-      <c r="AQ29" s="24"/>
-      <c r="AR29" s="24"/>
-      <c r="AS29" s="24"/>
-      <c r="AT29" s="24"/>
-      <c r="AU29" s="24"/>
-      <c r="AV29" s="24"/>
-      <c r="AW29" s="24"/>
-      <c r="AX29" s="24"/>
-      <c r="AY29" s="24"/>
-      <c r="AZ29" s="24"/>
-      <c r="BA29" s="24"/>
-      <c r="BB29" s="32"/>
-    </row>
-    <row r="30" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C30" s="43" t="s">
+      <c r="AZ28" s="43"/>
+    </row>
+    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A29" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="4"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2"/>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="2"/>
+      <c r="AE29" s="2"/>
+      <c r="AF29" s="2"/>
+      <c r="AG29" s="2"/>
+      <c r="AH29" s="2"/>
+      <c r="AI29" s="2"/>
+      <c r="AJ29" s="2"/>
+      <c r="AK29" s="2"/>
+      <c r="AL29" s="2"/>
+      <c r="AM29" s="2"/>
+      <c r="AN29" s="2"/>
+      <c r="AO29" s="2"/>
+      <c r="AP29" s="2"/>
+      <c r="AQ29" s="2"/>
+      <c r="AR29" s="2"/>
+      <c r="AS29" s="2"/>
+      <c r="AT29" s="2"/>
+      <c r="AU29" s="2"/>
+      <c r="AV29" s="2"/>
+      <c r="AW29" s="2"/>
+      <c r="AX29" s="2"/>
+      <c r="AY29" s="2"/>
+      <c r="AZ29" s="43"/>
+    </row>
+    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A30" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="32"/>
+      <c r="C30" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -2853,20 +2959,20 @@
       <c r="AW30" s="2"/>
       <c r="AX30" s="2"/>
       <c r="AY30" s="2"/>
-      <c r="AZ30" s="2"/>
-      <c r="BA30" s="2"/>
-      <c r="BB30" s="32"/>
-    </row>
-    <row r="31" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C31" s="43" t="s">
+      <c r="AZ30" s="43"/>
+    </row>
+    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A31" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="35"/>
-      <c r="E31" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F31" s="12"/>
-      <c r="G31" s="4"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -2911,20 +3017,20 @@
       <c r="AW31" s="2"/>
       <c r="AX31" s="2"/>
       <c r="AY31" s="2"/>
-      <c r="AZ31" s="2"/>
-      <c r="BA31" s="2"/>
-      <c r="BB31" s="32"/>
-    </row>
-    <row r="32" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C32" s="43" t="s">
+      <c r="AZ31" s="43"/>
+    </row>
+    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A32" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="4"/>
+      <c r="B32" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -2969,20 +3075,20 @@
       <c r="AW32" s="2"/>
       <c r="AX32" s="2"/>
       <c r="AY32" s="2"/>
-      <c r="AZ32" s="2"/>
-      <c r="BA32" s="2"/>
-      <c r="BB32" s="32"/>
-    </row>
-    <row r="33" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C33" s="43" t="s">
+      <c r="AZ32" s="43"/>
+    </row>
+    <row r="33" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A33" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="35"/>
-      <c r="E33" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="4"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -3027,20 +3133,20 @@
       <c r="AW33" s="2"/>
       <c r="AX33" s="2"/>
       <c r="AY33" s="2"/>
-      <c r="AZ33" s="2"/>
-      <c r="BA33" s="2"/>
-      <c r="BB33" s="32"/>
-    </row>
-    <row r="34" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C34" s="43" t="s">
+      <c r="AZ33" s="43"/>
+    </row>
+    <row r="34" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A34" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="4"/>
+      <c r="B34" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -3085,20 +3191,20 @@
       <c r="AW34" s="2"/>
       <c r="AX34" s="2"/>
       <c r="AY34" s="2"/>
-      <c r="AZ34" s="2"/>
-      <c r="BA34" s="2"/>
-      <c r="BB34" s="32"/>
-    </row>
-    <row r="35" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C35" s="43" t="s">
+      <c r="AZ34" s="43"/>
+    </row>
+    <row r="35" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A35" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="35"/>
-      <c r="E35" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="4"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="12"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -3143,20 +3249,20 @@
       <c r="AW35" s="2"/>
       <c r="AX35" s="2"/>
       <c r="AY35" s="2"/>
-      <c r="AZ35" s="2"/>
-      <c r="BA35" s="2"/>
-      <c r="BB35" s="32"/>
-    </row>
-    <row r="36" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C36" s="43" t="s">
+      <c r="AZ35" s="43"/>
+    </row>
+    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A36" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="4"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
@@ -3201,20 +3307,20 @@
       <c r="AW36" s="2"/>
       <c r="AX36" s="2"/>
       <c r="AY36" s="2"/>
-      <c r="AZ36" s="2"/>
-      <c r="BA36" s="2"/>
-      <c r="BB36" s="32"/>
-    </row>
-    <row r="37" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C37" s="43" t="s">
+      <c r="AZ36" s="43"/>
+    </row>
+    <row r="37" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A37" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="35"/>
-      <c r="E37" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="F37" s="12"/>
-      <c r="G37" s="4"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="12"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -3259,192 +3365,188 @@
       <c r="AW37" s="2"/>
       <c r="AX37" s="2"/>
       <c r="AY37" s="2"/>
-      <c r="AZ37" s="2"/>
-      <c r="BA37" s="2"/>
-      <c r="BB37" s="32"/>
-    </row>
-    <row r="38" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C38" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" s="35"/>
-      <c r="E38" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="F38" s="12"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="2"/>
-      <c r="U38" s="2"/>
-      <c r="V38" s="2"/>
-      <c r="W38" s="2"/>
-      <c r="X38" s="2"/>
-      <c r="Y38" s="2"/>
-      <c r="Z38" s="2"/>
-      <c r="AA38" s="2"/>
-      <c r="AB38" s="2"/>
-      <c r="AC38" s="2"/>
-      <c r="AD38" s="2"/>
-      <c r="AE38" s="2"/>
-      <c r="AF38" s="2"/>
-      <c r="AG38" s="2"/>
-      <c r="AH38" s="2"/>
-      <c r="AI38" s="2"/>
-      <c r="AJ38" s="2"/>
-      <c r="AK38" s="2"/>
-      <c r="AL38" s="2"/>
-      <c r="AM38" s="2"/>
-      <c r="AN38" s="2"/>
-      <c r="AO38" s="2"/>
-      <c r="AP38" s="2"/>
-      <c r="AQ38" s="2"/>
-      <c r="AR38" s="2"/>
-      <c r="AS38" s="2"/>
-      <c r="AT38" s="2"/>
-      <c r="AU38" s="2"/>
-      <c r="AV38" s="2"/>
-      <c r="AW38" s="2"/>
-      <c r="AX38" s="2"/>
-      <c r="AY38" s="2"/>
-      <c r="AZ38" s="2"/>
-      <c r="BA38" s="2"/>
-      <c r="BB38" s="32"/>
-    </row>
-    <row r="39" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C39" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="D39" s="35"/>
-      <c r="E39" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F39" s="12"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
-      <c r="W39" s="2"/>
-      <c r="X39" s="2"/>
-      <c r="Y39" s="2"/>
-      <c r="Z39" s="2"/>
-      <c r="AA39" s="2"/>
-      <c r="AB39" s="2"/>
-      <c r="AC39" s="2"/>
-      <c r="AD39" s="2"/>
-      <c r="AE39" s="2"/>
-      <c r="AF39" s="2"/>
-      <c r="AG39" s="2"/>
-      <c r="AH39" s="2"/>
-      <c r="AI39" s="2"/>
-      <c r="AJ39" s="2"/>
-      <c r="AK39" s="2"/>
-      <c r="AL39" s="2"/>
-      <c r="AM39" s="2"/>
-      <c r="AN39" s="2"/>
-      <c r="AO39" s="2"/>
-      <c r="AP39" s="2"/>
-      <c r="AQ39" s="2"/>
-      <c r="AR39" s="2"/>
-      <c r="AS39" s="2"/>
-      <c r="AT39" s="2"/>
-      <c r="AU39" s="2"/>
-      <c r="AV39" s="2"/>
-      <c r="AW39" s="2"/>
-      <c r="AX39" s="2"/>
-      <c r="AY39" s="2"/>
-      <c r="AZ39" s="2"/>
-      <c r="BA39" s="2"/>
-      <c r="BB39" s="32"/>
-    </row>
-    <row r="40" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C40" s="43" t="s">
+      <c r="AZ37" s="43"/>
+    </row>
+    <row r="38" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A38" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="37"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="28"/>
-      <c r="N40" s="28"/>
-      <c r="O40" s="28"/>
-      <c r="P40" s="28"/>
-      <c r="Q40" s="28"/>
-      <c r="R40" s="28"/>
-      <c r="S40" s="28"/>
-      <c r="T40" s="28"/>
-      <c r="U40" s="28"/>
-      <c r="V40" s="28"/>
-      <c r="W40" s="28"/>
-      <c r="X40" s="28"/>
-      <c r="Y40" s="28"/>
-      <c r="Z40" s="28"/>
-      <c r="AA40" s="28"/>
-      <c r="AB40" s="28"/>
-      <c r="AC40" s="28"/>
-      <c r="AD40" s="28"/>
-      <c r="AE40" s="28"/>
-      <c r="AF40" s="28"/>
-      <c r="AG40" s="28"/>
-      <c r="AH40" s="28"/>
-      <c r="AI40" s="28"/>
-      <c r="AJ40" s="28"/>
-      <c r="AK40" s="28"/>
-      <c r="AL40" s="28"/>
-      <c r="AM40" s="28"/>
-      <c r="AN40" s="28"/>
-      <c r="AO40" s="28"/>
-      <c r="AP40" s="28"/>
-      <c r="AQ40" s="28"/>
-      <c r="AR40" s="28"/>
-      <c r="AS40" s="28"/>
-      <c r="AT40" s="28"/>
-      <c r="AU40" s="28"/>
-      <c r="AV40" s="28"/>
-      <c r="AW40" s="28"/>
-      <c r="AX40" s="28"/>
-      <c r="AY40" s="28"/>
-      <c r="AZ40" s="28"/>
-      <c r="BA40" s="28"/>
-      <c r="BB40" s="32"/>
-    </row>
-    <row r="41" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C41" s="43" t="s">
+      <c r="B38" s="34"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
+      <c r="O38" s="28"/>
+      <c r="P38" s="28"/>
+      <c r="Q38" s="28"/>
+      <c r="R38" s="28"/>
+      <c r="S38" s="28"/>
+      <c r="T38" s="28"/>
+      <c r="U38" s="28"/>
+      <c r="V38" s="28"/>
+      <c r="W38" s="28"/>
+      <c r="X38" s="28"/>
+      <c r="Y38" s="28"/>
+      <c r="Z38" s="28"/>
+      <c r="AA38" s="28"/>
+      <c r="AB38" s="28"/>
+      <c r="AC38" s="28"/>
+      <c r="AD38" s="28"/>
+      <c r="AE38" s="28"/>
+      <c r="AF38" s="28"/>
+      <c r="AG38" s="28"/>
+      <c r="AH38" s="28"/>
+      <c r="AI38" s="28"/>
+      <c r="AJ38" s="28"/>
+      <c r="AK38" s="28"/>
+      <c r="AL38" s="28"/>
+      <c r="AM38" s="28"/>
+      <c r="AN38" s="28"/>
+      <c r="AO38" s="28"/>
+      <c r="AP38" s="28"/>
+      <c r="AQ38" s="28"/>
+      <c r="AR38" s="28"/>
+      <c r="AS38" s="28"/>
+      <c r="AT38" s="28"/>
+      <c r="AU38" s="28"/>
+      <c r="AV38" s="28"/>
+      <c r="AW38" s="28"/>
+      <c r="AX38" s="28"/>
+      <c r="AY38" s="28"/>
+      <c r="AZ38" s="43"/>
+    </row>
+    <row r="39" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A39" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="38" t="s">
+      <c r="B39" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="10"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="5"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
+      <c r="AA39" s="3"/>
+      <c r="AB39" s="3"/>
+      <c r="AC39" s="3"/>
+      <c r="AD39" s="3"/>
+      <c r="AE39" s="3"/>
+      <c r="AF39" s="3"/>
+      <c r="AG39" s="3"/>
+      <c r="AH39" s="3"/>
+      <c r="AI39" s="3"/>
+      <c r="AJ39" s="3"/>
+      <c r="AK39" s="3"/>
+      <c r="AL39" s="3"/>
+      <c r="AM39" s="3"/>
+      <c r="AN39" s="3"/>
+      <c r="AO39" s="3"/>
+      <c r="AP39" s="3"/>
+      <c r="AQ39" s="3"/>
+      <c r="AR39" s="3"/>
+      <c r="AS39" s="3"/>
+      <c r="AT39" s="3"/>
+      <c r="AU39" s="3"/>
+      <c r="AV39" s="3"/>
+      <c r="AW39" s="3"/>
+      <c r="AX39" s="3"/>
+      <c r="AY39" s="3"/>
+      <c r="AZ39" s="43"/>
+    </row>
+    <row r="40" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A40" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="35"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+      <c r="V40" s="3"/>
+      <c r="W40" s="3"/>
+      <c r="X40" s="3"/>
+      <c r="Y40" s="3"/>
+      <c r="Z40" s="3"/>
+      <c r="AA40" s="3"/>
+      <c r="AB40" s="3"/>
+      <c r="AC40" s="3"/>
+      <c r="AD40" s="3"/>
+      <c r="AE40" s="3"/>
+      <c r="AF40" s="3"/>
+      <c r="AG40" s="3"/>
+      <c r="AH40" s="3"/>
+      <c r="AI40" s="3"/>
+      <c r="AJ40" s="3"/>
+      <c r="AK40" s="3"/>
+      <c r="AL40" s="3"/>
+      <c r="AM40" s="3"/>
+      <c r="AN40" s="3"/>
+      <c r="AO40" s="3"/>
+      <c r="AP40" s="3"/>
+      <c r="AQ40" s="3"/>
+      <c r="AR40" s="3"/>
+      <c r="AS40" s="3"/>
+      <c r="AT40" s="3"/>
+      <c r="AU40" s="3"/>
+      <c r="AV40" s="3"/>
+      <c r="AW40" s="3"/>
+      <c r="AX40" s="3"/>
+      <c r="AY40" s="3"/>
+      <c r="AZ40" s="43"/>
+    </row>
+    <row r="41" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A41" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="36"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
@@ -3489,18 +3591,20 @@
       <c r="AW41" s="3"/>
       <c r="AX41" s="3"/>
       <c r="AY41" s="3"/>
-      <c r="AZ41" s="3"/>
-      <c r="BA41" s="3"/>
-      <c r="BB41" s="32"/>
-    </row>
-    <row r="42" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C42" s="43" t="s">
+      <c r="AZ41" s="43"/>
+    </row>
+    <row r="42" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A42" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="38"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="5"/>
+      <c r="B42" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
@@ -3545,18 +3649,18 @@
       <c r="AW42" s="3"/>
       <c r="AX42" s="3"/>
       <c r="AY42" s="3"/>
-      <c r="AZ42" s="3"/>
-      <c r="BA42" s="3"/>
-      <c r="BB42" s="32"/>
-    </row>
-    <row r="43" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C43" s="43" t="s">
+      <c r="AZ42" s="43"/>
+    </row>
+    <row r="43" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A43" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="D43" s="39"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="5"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
@@ -3601,20 +3705,18 @@
       <c r="AW43" s="3"/>
       <c r="AX43" s="3"/>
       <c r="AY43" s="3"/>
-      <c r="AZ43" s="3"/>
-      <c r="BA43" s="3"/>
-      <c r="BB43" s="32"/>
-    </row>
-    <row r="44" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C44" s="43" t="s">
+      <c r="AZ43" s="43"/>
+    </row>
+    <row r="44" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A44" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="E44" s="10"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="5"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
@@ -3659,18 +3761,20 @@
       <c r="AW44" s="3"/>
       <c r="AX44" s="3"/>
       <c r="AY44" s="3"/>
-      <c r="AZ44" s="3"/>
-      <c r="BA44" s="3"/>
-      <c r="BB44" s="32"/>
-    </row>
-    <row r="45" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C45" s="43" t="s">
+      <c r="AZ44" s="43"/>
+    </row>
+    <row r="45" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="D45" s="35"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="5"/>
+      <c r="B45" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
@@ -3715,128 +3819,12 @@
       <c r="AW45" s="3"/>
       <c r="AX45" s="3"/>
       <c r="AY45" s="3"/>
-      <c r="AZ45" s="3"/>
-      <c r="BA45" s="3"/>
-      <c r="BB45" s="32"/>
-    </row>
-    <row r="46" spans="3:54" x14ac:dyDescent="0.25">
-      <c r="C46" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="D46" s="38"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
-      <c r="V46" s="3"/>
-      <c r="W46" s="3"/>
-      <c r="X46" s="3"/>
-      <c r="Y46" s="3"/>
-      <c r="Z46" s="3"/>
-      <c r="AA46" s="3"/>
-      <c r="AB46" s="3"/>
-      <c r="AC46" s="3"/>
-      <c r="AD46" s="3"/>
-      <c r="AE46" s="3"/>
-      <c r="AF46" s="3"/>
-      <c r="AG46" s="3"/>
-      <c r="AH46" s="3"/>
-      <c r="AI46" s="3"/>
-      <c r="AJ46" s="3"/>
-      <c r="AK46" s="3"/>
-      <c r="AL46" s="3"/>
-      <c r="AM46" s="3"/>
-      <c r="AN46" s="3"/>
-      <c r="AO46" s="3"/>
-      <c r="AP46" s="3"/>
-      <c r="AQ46" s="3"/>
-      <c r="AR46" s="3"/>
-      <c r="AS46" s="3"/>
-      <c r="AT46" s="3"/>
-      <c r="AU46" s="3"/>
-      <c r="AV46" s="3"/>
-      <c r="AW46" s="3"/>
-      <c r="AX46" s="3"/>
-      <c r="AY46" s="3"/>
-      <c r="AZ46" s="3"/>
-      <c r="BA46" s="3"/>
-      <c r="BB46" s="32"/>
-    </row>
-    <row r="47" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="D47" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="E47" s="15"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-      <c r="O47" s="3"/>
-      <c r="P47" s="3"/>
-      <c r="Q47" s="3"/>
-      <c r="R47" s="3"/>
-      <c r="S47" s="3"/>
-      <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
-      <c r="V47" s="3"/>
-      <c r="W47" s="3"/>
-      <c r="X47" s="3"/>
-      <c r="Y47" s="3"/>
-      <c r="Z47" s="3"/>
-      <c r="AA47" s="3"/>
-      <c r="AB47" s="3"/>
-      <c r="AC47" s="3"/>
-      <c r="AD47" s="3"/>
-      <c r="AE47" s="3"/>
-      <c r="AF47" s="3"/>
-      <c r="AG47" s="3"/>
-      <c r="AH47" s="3"/>
-      <c r="AI47" s="3"/>
-      <c r="AJ47" s="3"/>
-      <c r="AK47" s="3"/>
-      <c r="AL47" s="3"/>
-      <c r="AM47" s="3"/>
-      <c r="AN47" s="3"/>
-      <c r="AO47" s="3"/>
-      <c r="AP47" s="3"/>
-      <c r="AQ47" s="3"/>
-      <c r="AR47" s="3"/>
-      <c r="AS47" s="3"/>
-      <c r="AT47" s="3"/>
-      <c r="AU47" s="3"/>
-      <c r="AV47" s="3"/>
-      <c r="AW47" s="3"/>
-      <c r="AX47" s="3"/>
-      <c r="AY47" s="3"/>
-      <c r="AZ47" s="3"/>
-      <c r="BA47" s="3"/>
-      <c r="BB47" s="33"/>
-    </row>
-    <row r="48" spans="3:54" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="AZ45" s="44"/>
+    </row>
+    <row r="46" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="BB4:BB47"/>
+    <mergeCell ref="AZ2:AZ45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>